<commit_message>
Fixed wrong model names in the region_aggregation tab.
</commit_message>
<xml_diff>
--- a/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-MAgPIE_2.1-4.2.xlsx
+++ b/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-MAgPIE_2.1-4.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -92,7 +92,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>BS</author>
+    <author>AD</author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0">
@@ -180,7 +180,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>BS</author>
+    <author>AD</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -243,7 +243,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>BS</author>
+    <author>AD</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="1037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="1036">
   <si>
     <t xml:space="preserve">General Instructions</t>
   </si>
@@ -3410,9 +3410,6 @@
   </si>
   <si>
     <t xml:space="preserve">Standardized Region Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REMIND-EDGET 2.1</t>
   </si>
   <si>
     <t xml:space="preserve">Native Region Name</t>
@@ -4106,7 +4103,7 @@
   <dimension ref="A1:N316"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A3:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7115,7 +7112,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="A3:A32 E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7492,8 +7489,8 @@
   </sheetPr>
   <dimension ref="A1:MQ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AR14" activeCellId="1" sqref="A3:A32 AR14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11753,7 +11750,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A3:A32 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11926,8 +11923,8 @@
   </sheetPr>
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11958,7 +11955,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B3" s="65" t="s">
         <v>1021</v>
@@ -11969,7 +11966,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B4" s="65" t="s">
         <v>1018</v>
@@ -11980,7 +11977,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B5" s="65" t="s">
         <v>1010</v>
@@ -11991,7 +11988,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B6" s="65" t="s">
         <v>288</v>
@@ -12002,7 +11999,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B7" s="65" t="s">
         <v>1024</v>
@@ -12013,7 +12010,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B8" s="65" t="s">
         <v>1012</v>
@@ -12024,7 +12021,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B9" s="65" t="s">
         <v>310</v>
@@ -12035,7 +12032,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B10" s="65" t="s">
         <v>546</v>
@@ -12046,7 +12043,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B11" s="65" t="s">
         <v>1026</v>
@@ -12057,7 +12054,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B12" s="65" t="s">
         <v>1028</v>
@@ -12068,7 +12065,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B13" s="65" t="s">
         <v>1016</v>
@@ -12079,7 +12076,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B14" s="65" t="s">
         <v>1020</v>
@@ -12090,7 +12087,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B15" s="65" t="s">
         <v>546</v>
@@ -12101,7 +12098,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B16" s="65" t="s">
         <v>1012</v>
@@ -12112,7 +12109,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B17" s="65" t="s">
         <v>1010</v>
@@ -12123,7 +12120,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B18" s="65" t="s">
         <v>288</v>
@@ -12134,7 +12131,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B19" s="65" t="s">
         <v>1020</v>
@@ -12145,7 +12142,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B20" s="65" t="s">
         <v>310</v>
@@ -12156,7 +12153,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B21" s="65" t="s">
         <v>1010</v>
@@ -12167,7 +12164,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B22" s="65" t="s">
         <v>1012</v>
@@ -12178,7 +12175,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B23" s="65" t="s">
         <v>288</v>
@@ -12189,7 +12186,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B24" s="65" t="s">
         <v>310</v>
@@ -12200,7 +12197,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B25" s="65" t="s">
         <v>1016</v>
@@ -12211,7 +12208,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B26" s="65" t="s">
         <v>1018</v>
@@ -12222,7 +12219,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B27" s="65" t="s">
         <v>1020</v>
@@ -12233,7 +12230,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B28" s="65" t="s">
         <v>1021</v>
@@ -12244,7 +12241,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B29" s="65" t="s">
         <v>546</v>
@@ -12255,7 +12252,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B30" s="65" t="s">
         <v>1024</v>
@@ -12266,7 +12263,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B31" s="65" t="s">
         <v>1026</v>
@@ -12277,7 +12274,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="64" t="s">
-        <v>1033</v>
+        <v>589</v>
       </c>
       <c r="B32" s="65" t="s">
         <v>1028</v>
@@ -12308,7 +12305,7 @@
   <dimension ref="A1:J249"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+      <selection pane="topLeft" activeCell="L8" activeCellId="1" sqref="A3:A32 L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12324,13 +12321,13 @@
         <v>1008</v>
       </c>
       <c r="B1" s="67" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1034</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>1035</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>1036</v>
       </c>
       <c r="I1" s="0"/>
     </row>

</xml_diff>

<commit_message>
fixed R10 regional aggregation for R2.1-M4.2: JPN -> R10PAC_OECD (not OECD)
</commit_message>
<xml_diff>
--- a/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-MAgPIE_2.1-4.2.xlsx
+++ b/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-MAgPIE_2.1-4.2.xlsx
@@ -92,7 +92,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>AD</author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0">
@@ -180,7 +180,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>AD</author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -243,7 +243,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>AD</author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -4103,7 +4103,7 @@
   <dimension ref="A1:N316"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A3:A32"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7112,7 +7112,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="A3:A32 E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7490,7 +7490,7 @@
   <dimension ref="A1:MQ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AR14" activeCellId="1" sqref="A3:A32 AR14"/>
+      <selection pane="topLeft" activeCell="AR14" activeCellId="0" sqref="AR14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11750,7 +11750,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A3:A32 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11924,7 +11924,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A32"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12192,7 +12192,7 @@
         <v>310</v>
       </c>
       <c r="C24" s="68" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12305,7 +12305,7 @@
   <dimension ref="A1:J249"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="1" sqref="A3:A32 L8"/>
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>